<commit_message>
Forgot to update my time log
</commit_message>
<xml_diff>
--- a/Sprint 3/Sprint 3 Hours Log -- Mason.xlsx
+++ b/Sprint 3/Sprint 3 Hours Log -- Mason.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Date</t>
   </si>
@@ -54,22 +54,21 @@
   </si>
   <si>
     <t>Changed the way we save top scores to a text file</t>
+  </si>
+  <si>
+    <t>SF-17</t>
+  </si>
+  <si>
+    <t>Almost finished everything for this user story. All that is left is a sort method for the model</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -182,21 +181,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="14" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -540,7 +536,7 @@
   <dimension ref="A1:D34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -572,10 +568,10 @@
       <c r="B2" s="3">
         <v>1.5</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="C2" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="12" t="s">
+      <c r="D2" s="10" t="s">
         <v>5</v>
       </c>
     </row>
@@ -586,54 +582,62 @@
       <c r="B3" s="3">
         <v>3</v>
       </c>
-      <c r="C3" s="13" t="s">
+      <c r="C3" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="13" t="s">
+      <c r="D3" s="11" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A4" s="2"/>
-      <c r="B4" s="3"/>
-      <c r="C4" s="6"/>
-      <c r="D4" s="5"/>
+      <c r="A4" s="2">
+        <v>42844</v>
+      </c>
+      <c r="B4" s="3">
+        <v>3</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="12" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="5" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="2"/>
       <c r="B5" s="3"/>
-      <c r="C5" s="7"/>
-      <c r="D5" s="7"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
     </row>
     <row r="6" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="2"/>
       <c r="B6" s="3"/>
-      <c r="C6" s="7"/>
-      <c r="D6" s="7"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
     </row>
     <row r="7" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="2"/>
       <c r="B7" s="3"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="8"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
     </row>
     <row r="8" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="2"/>
       <c r="B8" s="3"/>
-      <c r="C8" s="9"/>
-      <c r="D8" s="9"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
     </row>
     <row r="9" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="2"/>
       <c r="B9" s="3"/>
-      <c r="C9" s="10"/>
-      <c r="D9" s="10"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
     </row>
     <row r="10" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="2"/>
       <c r="B10" s="3"/>
-      <c r="C10" s="11"/>
-      <c r="D10" s="11"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="9"/>
     </row>
     <row r="11" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="3"/>

</xml_diff>

<commit_message>
Updated time log and text file of To-Dos
</commit_message>
<xml_diff>
--- a/Sprint 3/Sprint 3 Hours Log -- Mason.xlsx
+++ b/Sprint 3/Sprint 3 Hours Log -- Mason.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
   <si>
     <t>Date</t>
   </si>
@@ -60,15 +60,25 @@
   </si>
   <si>
     <t>Almost finished everything for this user story. All that is left is a sort method for the model</t>
+  </si>
+  <si>
+    <t>Created the sort method and properly implemented it</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -181,18 +191,21 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -536,7 +549,7 @@
   <dimension ref="A1:D34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -604,10 +617,18 @@
       </c>
     </row>
     <row r="5" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A5" s="2"/>
-      <c r="B5" s="3"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
+      <c r="A5" s="2">
+        <v>42845</v>
+      </c>
+      <c r="B5" s="3">
+        <v>1</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="13" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="6" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="2"/>

</xml_diff>

<commit_message>
Finished the top ten lists! Dates are added and they are sorting and saving properly.
</commit_message>
<xml_diff>
--- a/Sprint 3/Sprint 3 Hours Log -- Mason.xlsx
+++ b/Sprint 3/Sprint 3 Hours Log -- Mason.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
   <si>
     <t>Date</t>
   </si>
@@ -63,6 +63,9 @@
   </si>
   <si>
     <t>Created the sort method and properly implemented it</t>
+  </si>
+  <si>
+    <t>Added the date to both top ten lists</t>
   </si>
 </sst>
 </file>
@@ -549,7 +552,7 @@
   <dimension ref="A1:D34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -581,10 +584,10 @@
       <c r="B2" s="3">
         <v>1.5</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="C2" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="D2" s="9" t="s">
         <v>5</v>
       </c>
     </row>
@@ -595,10 +598,10 @@
       <c r="B3" s="3">
         <v>3</v>
       </c>
-      <c r="C3" s="11" t="s">
+      <c r="C3" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="11" t="s">
+      <c r="D3" s="10" t="s">
         <v>7</v>
       </c>
     </row>
@@ -609,10 +612,10 @@
       <c r="B4" s="3">
         <v>3</v>
       </c>
-      <c r="C4" s="12" t="s">
+      <c r="C4" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="12" t="s">
+      <c r="D4" s="11" t="s">
         <v>9</v>
       </c>
     </row>
@@ -623,42 +626,50 @@
       <c r="B5" s="3">
         <v>1</v>
       </c>
-      <c r="C5" s="13" t="s">
+      <c r="C5" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="13" t="s">
+      <c r="D5" s="12" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A6" s="2"/>
-      <c r="B6" s="3"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
+      <c r="A6" s="2">
+        <v>42845</v>
+      </c>
+      <c r="B6" s="3">
+        <v>1.5</v>
+      </c>
+      <c r="C6" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="13" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="7" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="2"/>
       <c r="B7" s="3"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
     </row>
     <row r="8" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="2"/>
       <c r="B8" s="3"/>
-      <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
     </row>
     <row r="9" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="2"/>
       <c r="B9" s="3"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="8"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
     </row>
     <row r="10" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="2"/>
       <c r="B10" s="3"/>
-      <c r="C10" s="9"/>
-      <c r="D10" s="9"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
     </row>
     <row r="11" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="3"/>

</xml_diff>

<commit_message>
Added the button for tile removal of a certain number. SF-13
</commit_message>
<xml_diff>
--- a/Sprint 3/Sprint 3 Hours Log -- Mason.xlsx
+++ b/Sprint 3/Sprint 3 Hours Log -- Mason.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
   <si>
     <t>Date</t>
   </si>
@@ -66,6 +66,12 @@
   </si>
   <si>
     <t>Added the date to both top ten lists</t>
+  </si>
+  <si>
+    <t>SF-13</t>
+  </si>
+  <si>
+    <t>Added a button that will remove all tiles of a number based on user input</t>
   </si>
 </sst>
 </file>
@@ -552,7 +558,7 @@
   <dimension ref="A1:D34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -584,10 +590,10 @@
       <c r="B2" s="3">
         <v>1.5</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="C2" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="D2" s="8" t="s">
         <v>5</v>
       </c>
     </row>
@@ -598,10 +604,10 @@
       <c r="B3" s="3">
         <v>3</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="C3" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="10" t="s">
+      <c r="D3" s="9" t="s">
         <v>7</v>
       </c>
     </row>
@@ -612,10 +618,10 @@
       <c r="B4" s="3">
         <v>3</v>
       </c>
-      <c r="C4" s="11" t="s">
+      <c r="C4" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="11" t="s">
+      <c r="D4" s="10" t="s">
         <v>9</v>
       </c>
     </row>
@@ -626,10 +632,10 @@
       <c r="B5" s="3">
         <v>1</v>
       </c>
-      <c r="C5" s="12" t="s">
+      <c r="C5" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="12" t="s">
+      <c r="D5" s="11" t="s">
         <v>10</v>
       </c>
     </row>
@@ -640,36 +646,44 @@
       <c r="B6" s="3">
         <v>1.5</v>
       </c>
-      <c r="C6" s="13" t="s">
+      <c r="C6" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="13" t="s">
+      <c r="D6" s="12" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A7" s="2"/>
-      <c r="B7" s="3"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
+      <c r="A7" s="2">
+        <v>42845</v>
+      </c>
+      <c r="B7" s="3">
+        <v>1</v>
+      </c>
+      <c r="C7" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" s="13" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="8" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="2"/>
       <c r="B8" s="3"/>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
     </row>
     <row r="9" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="2"/>
       <c r="B9" s="3"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="7"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
     </row>
     <row r="10" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="2"/>
       <c r="B10" s="3"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="8"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
     </row>
     <row r="11" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="3"/>

</xml_diff>

<commit_message>
Updated time log and text file for remaining user stories.
</commit_message>
<xml_diff>
--- a/Sprint 3/Sprint 3 Hours Log -- Mason.xlsx
+++ b/Sprint 3/Sprint 3 Hours Log -- Mason.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
   <si>
     <t>Date</t>
   </si>
@@ -72,6 +72,12 @@
   </si>
   <si>
     <t>Added a button that will remove all tiles of a number based on user input</t>
+  </si>
+  <si>
+    <t>SF-13 &amp; SF-14</t>
+  </si>
+  <si>
+    <t>Made the changes for the limit on how often you can use these features</t>
   </si>
 </sst>
 </file>
@@ -558,7 +564,7 @@
   <dimension ref="A1:D34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -590,10 +596,10 @@
       <c r="B2" s="3">
         <v>1.5</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="7" t="s">
         <v>5</v>
       </c>
     </row>
@@ -604,10 +610,10 @@
       <c r="B3" s="3">
         <v>3</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="C3" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="D3" s="8" t="s">
         <v>7</v>
       </c>
     </row>
@@ -618,10 +624,10 @@
       <c r="B4" s="3">
         <v>3</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="C4" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="10" t="s">
+      <c r="D4" s="9" t="s">
         <v>9</v>
       </c>
     </row>
@@ -632,10 +638,10 @@
       <c r="B5" s="3">
         <v>1</v>
       </c>
-      <c r="C5" s="11" t="s">
+      <c r="C5" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="11" t="s">
+      <c r="D5" s="10" t="s">
         <v>10</v>
       </c>
     </row>
@@ -646,10 +652,10 @@
       <c r="B6" s="3">
         <v>1.5</v>
       </c>
-      <c r="C6" s="12" t="s">
+      <c r="C6" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="12" t="s">
+      <c r="D6" s="11" t="s">
         <v>11</v>
       </c>
     </row>
@@ -660,30 +666,38 @@
       <c r="B7" s="3">
         <v>1</v>
       </c>
-      <c r="C7" s="13" t="s">
+      <c r="C7" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="D7" s="13" t="s">
+      <c r="D7" s="12" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A8" s="2"/>
-      <c r="B8" s="3"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
+      <c r="A8" s="2">
+        <v>42848</v>
+      </c>
+      <c r="B8" s="3">
+        <v>1</v>
+      </c>
+      <c r="C8" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8" s="13" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="9" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="2"/>
       <c r="B9" s="3"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
     </row>
     <row r="10" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="2"/>
       <c r="B10" s="3"/>
-      <c r="C10" s="7"/>
-      <c r="D10" s="7"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
     </row>
     <row r="11" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="3"/>

</xml_diff>